<commit_message>
update ref luong cua Phu tại CAN THO
</commit_message>
<xml_diff>
--- a/Ref tính lương.xlsx
+++ b/Ref tính lương.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\3_CODING\Python\NotionAPI\git\Notion_API_with_python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CB3E2FA-60CC-4919-BED9-04E57E069498}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24A79F4F-6809-4017-B585-A8073E191316}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-30" yWindow="-16320" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-30" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Lương cơ bản" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="162">
   <si>
     <t>notion id</t>
   </si>
@@ -438,9 +438,6 @@
   </si>
   <si>
     <t>Số tháng</t>
-  </si>
-  <si>
-    <t>Phụ cấp</t>
   </si>
   <si>
     <t>Nhóm dịch vụ</t>
@@ -863,11 +860,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U27"/>
+  <dimension ref="A1:T27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="4" topLeftCell="P1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="Q35" sqref="Q35"/>
+      <selection pane="topRight" activeCell="T10" sqref="T10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -889,13 +886,12 @@
     <col min="15" max="15" width="9.453125" customWidth="1"/>
     <col min="16" max="16" width="15.453125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="16.81640625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.36328125" customWidth="1"/>
-    <col min="19" max="19" width="8.453125" style="2" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.6328125" style="2" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="10.6328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="8.453125" style="2" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.6328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10.6328125" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -947,20 +943,17 @@
       <c r="Q1" t="s">
         <v>132</v>
       </c>
-      <c r="R1" t="s">
-        <v>134</v>
+      <c r="R1" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="S1" s="2" t="s">
-        <v>22</v>
+        <v>85</v>
       </c>
       <c r="T1" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="U1" s="2" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -1015,11 +1008,8 @@
         <f ca="1">N2+P2</f>
         <v>0</v>
       </c>
-      <c r="R2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>25</v>
       </c>
@@ -1074,11 +1064,8 @@
         <f t="shared" ref="Q3:Q27" ca="1" si="2">N3+P3</f>
         <v>0</v>
       </c>
-      <c r="R3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.35">
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>33</v>
       </c>
@@ -1118,11 +1105,8 @@
         <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
-      <c r="R4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.35">
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>37</v>
       </c>
@@ -1174,14 +1158,11 @@
         <f t="shared" ca="1" si="2"/>
         <v>7840000</v>
       </c>
-      <c r="R5">
-        <v>1000000</v>
-      </c>
-      <c r="S5" s="2">
+      <c r="R5" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>46</v>
       </c>
@@ -1224,23 +1205,20 @@
         <f t="shared" ca="1" si="2"/>
         <v>11500000</v>
       </c>
-      <c r="R6">
-        <v>0</v>
-      </c>
-      <c r="S6" s="2">
+      <c r="R6" s="2">
         <f>1/3</f>
         <v>0.33333333333333331</v>
       </c>
+      <c r="S6" s="2">
+        <f t="shared" ref="S6:T7" si="3">1/3</f>
+        <v>0.33333333333333331</v>
+      </c>
       <c r="T6" s="2">
-        <f t="shared" ref="T6:U7" si="3">1/3</f>
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="U6" s="2">
         <f t="shared" si="3"/>
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>50</v>
       </c>
@@ -1283,23 +1261,20 @@
         <f t="shared" ca="1" si="2"/>
         <v>9270000</v>
       </c>
-      <c r="R7">
-        <v>0</v>
+      <c r="R7" s="2">
+        <f>1/3</f>
+        <v>0.33333333333333331</v>
       </c>
       <c r="S7" s="2">
         <f>1/3</f>
         <v>0.33333333333333331</v>
       </c>
       <c r="T7" s="2">
-        <f>1/3</f>
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="U7" s="2">
         <f t="shared" si="3"/>
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>54</v>
       </c>
@@ -1342,19 +1317,16 @@
         <f t="shared" ca="1" si="2"/>
         <v>28750000</v>
       </c>
-      <c r="R8">
-        <v>0</v>
-      </c>
-      <c r="T8" s="2">
+      <c r="S8" s="2">
         <f>10/25</f>
         <v>0.4</v>
       </c>
-      <c r="U8" s="2">
+      <c r="T8" s="2">
         <f>15/25</f>
         <v>0.6</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>56</v>
       </c>
@@ -1403,14 +1375,11 @@
         <f t="shared" ca="1" si="2"/>
         <v>9810000</v>
       </c>
-      <c r="R9">
-        <v>1000000</v>
-      </c>
-      <c r="U9" s="2">
+      <c r="T9" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>63</v>
       </c>
@@ -1459,14 +1428,11 @@
         <f t="shared" ca="1" si="2"/>
         <v>4500000</v>
       </c>
-      <c r="R10">
-        <v>1000000</v>
-      </c>
-      <c r="S10" s="2">
+      <c r="R10" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>68</v>
       </c>
@@ -1515,23 +1481,20 @@
         <f t="shared" ca="1" si="2"/>
         <v>8000000</v>
       </c>
-      <c r="R11">
-        <v>0</v>
-      </c>
-      <c r="S11" s="2">
+      <c r="R11" s="2">
         <f>3/8</f>
         <v>0.375</v>
       </c>
-      <c r="T11" s="2">
+      <c r="S11" s="2">
         <f>2/8</f>
         <v>0.25</v>
       </c>
-      <c r="U11" s="2">
+      <c r="T11" s="2">
         <f>3/8</f>
         <v>0.375</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>73</v>
       </c>
@@ -1580,14 +1543,11 @@
         <f t="shared" ca="1" si="2"/>
         <v>5665000</v>
       </c>
-      <c r="R12">
-        <v>0</v>
-      </c>
-      <c r="U12" s="2">
+      <c r="T12" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>78</v>
       </c>
@@ -1627,11 +1587,8 @@
         <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
-      <c r="R13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.35">
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>80</v>
       </c>
@@ -1680,14 +1637,11 @@
         <f t="shared" ca="1" si="2"/>
         <v>8480000</v>
       </c>
-      <c r="R14">
-        <v>1000000</v>
-      </c>
-      <c r="T14" s="2">
+      <c r="S14" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>86</v>
       </c>
@@ -1736,14 +1690,11 @@
         <f t="shared" ca="1" si="2"/>
         <v>4000000</v>
       </c>
-      <c r="R15">
-        <v>1000000</v>
-      </c>
-      <c r="T15" s="2">
+      <c r="S15" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>91</v>
       </c>
@@ -1792,14 +1743,11 @@
         <f t="shared" ca="1" si="2"/>
         <v>4120000</v>
       </c>
-      <c r="R16">
-        <v>1000000</v>
-      </c>
-      <c r="U16" s="2">
+      <c r="T16" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>96</v>
       </c>
@@ -1842,14 +1790,11 @@
         <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
-      <c r="R17">
-        <v>0</v>
-      </c>
-      <c r="S17" s="2">
+      <c r="R17" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>98</v>
       </c>
@@ -1895,14 +1840,11 @@
         <f t="shared" ca="1" si="2"/>
         <v>3000000</v>
       </c>
-      <c r="R18">
-        <v>1000000</v>
-      </c>
-      <c r="U18" s="2">
+      <c r="R18" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>100</v>
       </c>
@@ -1951,14 +1893,11 @@
         <f t="shared" ca="1" si="2"/>
         <v>3000000</v>
       </c>
-      <c r="R19">
-        <v>1000000</v>
-      </c>
-      <c r="T19" s="2">
+      <c r="S19" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>103</v>
       </c>
@@ -2001,23 +1940,20 @@
         <f t="shared" ca="1" si="2"/>
         <v>8240000</v>
       </c>
-      <c r="R20">
-        <v>0</v>
-      </c>
-      <c r="S20" s="2">
+      <c r="R20" s="2">
         <f>2/8</f>
         <v>0.25</v>
+      </c>
+      <c r="S20" s="2">
+        <f>3/8</f>
+        <v>0.375</v>
       </c>
       <c r="T20" s="2">
         <f>3/8</f>
         <v>0.375</v>
       </c>
-      <c r="U20" s="2">
-        <f>3/8</f>
-        <v>0.375</v>
-      </c>
-    </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.35">
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>105</v>
       </c>
@@ -2054,11 +1990,8 @@
         <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
-      <c r="R21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.35">
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>107</v>
       </c>
@@ -2092,14 +2025,11 @@
         <f t="shared" ca="1" si="2"/>
         <v>6000000</v>
       </c>
-      <c r="R22">
-        <v>0</v>
-      </c>
-      <c r="S22" s="2">
+      <c r="R22" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>109</v>
       </c>
@@ -2148,14 +2078,11 @@
         <f t="shared" ca="1" si="2"/>
         <v>5000000</v>
       </c>
-      <c r="R23">
-        <v>1000000</v>
-      </c>
-      <c r="T23" s="2">
+      <c r="S23" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>115</v>
       </c>
@@ -2192,11 +2119,8 @@
         <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
-      <c r="R24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.35">
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>117</v>
       </c>
@@ -2245,14 +2169,11 @@
         <f t="shared" ca="1" si="2"/>
         <v>3000000</v>
       </c>
-      <c r="R25">
-        <v>0</v>
-      </c>
-      <c r="U25" s="2">
+      <c r="T25" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>122</v>
       </c>
@@ -2301,11 +2222,8 @@
         <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
-      <c r="R26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.35">
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>128</v>
       </c>
@@ -2345,10 +2263,7 @@
         <f t="shared" ca="1" si="2"/>
         <v>3000000</v>
       </c>
-      <c r="R27">
-        <v>0</v>
-      </c>
-      <c r="T27" s="2">
+      <c r="S27" s="2">
         <v>1</v>
       </c>
     </row>
@@ -2361,7 +2276,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D194953-9D63-4E72-B6A9-71562AC783DD}">
   <dimension ref="A1:S14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="C21" sqref="C21"/>
     </sheetView>
@@ -2376,66 +2291,66 @@
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="L1" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="M1" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="N1" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="O1" s="5" t="s">
         <v>154</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="P1" s="5" t="s">
         <v>155</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="Q1" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="R1" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="S1" s="4" t="s">
         <v>158</v>
-      </c>
-      <c r="S1" s="4" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B2">
         <v>0.1</v>
@@ -2494,7 +2409,7 @@
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B3">
         <v>0.1</v>
@@ -2553,7 +2468,7 @@
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B4">
         <v>0.1</v>
@@ -2612,7 +2527,7 @@
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B5">
         <v>7.0000000000000007E-2</v>
@@ -2671,7 +2586,7 @@
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B6">
         <v>0.1</v>
@@ -2718,7 +2633,7 @@
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B7">
         <v>0.1</v>
@@ -2777,7 +2692,7 @@
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B8">
         <v>0.1</v>
@@ -2824,7 +2739,7 @@
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B9">
         <v>0.1</v>
@@ -2883,7 +2798,7 @@
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B10">
         <v>0</v>

</xml_diff>

<commit_message>
update ref luong cho 3 nguoi o LX
</commit_message>
<xml_diff>
--- a/Ref tính lương.xlsx
+++ b/Ref tính lương.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\3_CODING\Python\NotionAPI\git\Notion_API_with_python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98ED266F-5ABF-4F98-964D-B6BCE8E92965}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{504389C7-37BA-4478-881B-ADFBF7034AF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-30" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Lương cơ bản" sheetId="1" r:id="rId1"/>
@@ -826,11 +826,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:S26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="4" topLeftCell="M1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="T22" sqref="T22"/>
+      <pane xSplit="4" topLeftCell="K1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="R21" sqref="R21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -914,7 +915,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:19" hidden="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -949,7 +950,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:19" hidden="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>24</v>
       </c>
@@ -999,7 +1000,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:19" hidden="1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>33</v>
       </c>
@@ -1049,7 +1050,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:19" hidden="1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>37</v>
       </c>
@@ -1099,7 +1100,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:19" hidden="1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>41</v>
       </c>
@@ -1146,7 +1147,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:19" hidden="1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>43</v>
       </c>
@@ -1193,7 +1194,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:19" hidden="1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>50</v>
       </c>
@@ -1240,7 +1241,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:19" hidden="1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>55</v>
       </c>
@@ -1296,7 +1297,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:19" hidden="1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>60</v>
       </c>
@@ -1343,7 +1344,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:19" hidden="1" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>65</v>
       </c>
@@ -1419,7 +1420,7 @@
         <v>1</v>
       </c>
       <c r="R12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S12">
         <v>0</v>
@@ -1466,13 +1467,13 @@
         <v>1</v>
       </c>
       <c r="R13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S13">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:19" hidden="1" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>78</v>
       </c>
@@ -1519,7 +1520,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:19" hidden="1" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>83</v>
       </c>
@@ -1560,7 +1561,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:19" hidden="1" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>85</v>
       </c>
@@ -1645,13 +1646,13 @@
         <v>1</v>
       </c>
       <c r="R17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S17">
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:19" hidden="1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>90</v>
       </c>
@@ -1701,7 +1702,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:19" hidden="1" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>92</v>
       </c>
@@ -1733,7 +1734,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:19" hidden="1" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>94</v>
       </c>
@@ -1812,7 +1813,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:19" hidden="1" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>102</v>
       </c>
@@ -1844,7 +1845,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:19" hidden="1" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>104</v>
       </c>
@@ -1891,7 +1892,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:19" hidden="1" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>109</v>
       </c>
@@ -1973,7 +1974,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:19" hidden="1" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>146</v>
       </c>
@@ -2012,7 +2013,13 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:R26" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:R26" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="10">
+      <filters>
+        <filter val="LONG XUYÊN"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>